<commit_message>
Update dtw excel results
</commit_message>
<xml_diff>
--- a/Saved Model/full_eeg/dtw_results.xlsx
+++ b/Saved Model/full_eeg/dtw_results.xlsx
@@ -8,7 +8,8 @@
     <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Foglio1" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Riassunto" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Subj 2" sheetId="2" state="visible" r:id="rId3"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -306,8 +307,8 @@
   </sheetPr>
   <dimension ref="A1:KE26"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D28" activeCellId="0" sqref="D28"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D4" activeCellId="0" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.90234375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1942,788 +1943,788 @@
       </c>
       <c r="B4" s="7" t="n">
         <f aca="false">AVERAGE(D4:AAA4)</f>
-        <v>2.78558725868726</v>
+        <v>2.11785818532819</v>
       </c>
       <c r="C4" s="8" t="n">
         <f aca="false">_xlfn.STDEV.S(D4:AAB4)</f>
-        <v>1.34833323396875</v>
+        <v>0.984302234813625</v>
       </c>
       <c r="D4" s="5" t="n">
-        <v>4.20189</v>
+        <v>1.94361</v>
       </c>
       <c r="E4" s="5" t="n">
-        <v>1.9969</v>
+        <v>2.2246</v>
       </c>
       <c r="F4" s="5" t="n">
-        <v>2.33531</v>
+        <v>3.54018</v>
       </c>
       <c r="G4" s="5" t="n">
-        <v>3.01635</v>
+        <v>1.25453</v>
       </c>
       <c r="H4" s="5" t="n">
-        <v>1.85524</v>
+        <v>2.97138</v>
       </c>
       <c r="I4" s="5" t="n">
-        <v>2.0973</v>
+        <v>3.39462</v>
       </c>
       <c r="J4" s="5" t="n">
-        <v>1.56276</v>
+        <v>3.19647</v>
       </c>
       <c r="K4" s="5" t="n">
-        <v>1.74056</v>
+        <v>1.29214</v>
       </c>
       <c r="L4" s="5" t="n">
-        <v>2.62222</v>
+        <v>2.64716</v>
       </c>
       <c r="M4" s="5" t="n">
-        <v>3.5979</v>
+        <v>2.28429</v>
       </c>
       <c r="N4" s="5" t="n">
-        <v>1.6625</v>
+        <v>1.47643</v>
       </c>
       <c r="O4" s="5" t="n">
-        <v>1.3376</v>
+        <v>1.48044</v>
       </c>
       <c r="P4" s="5" t="n">
-        <v>1.86845</v>
+        <v>1.43405</v>
       </c>
       <c r="Q4" s="5" t="n">
-        <v>3.882</v>
+        <v>2.289</v>
       </c>
       <c r="R4" s="5" t="n">
-        <v>2.67362</v>
+        <v>3.37076</v>
       </c>
       <c r="S4" s="5" t="n">
-        <v>2.87823</v>
+        <v>3.61145</v>
       </c>
       <c r="T4" s="5" t="n">
-        <v>1.93722</v>
+        <v>1.57736</v>
       </c>
       <c r="U4" s="5" t="n">
-        <v>2.13169</v>
+        <v>3.61217</v>
       </c>
       <c r="V4" s="5" t="n">
-        <v>1.55793</v>
+        <v>2.36538</v>
       </c>
       <c r="W4" s="5" t="n">
-        <v>3.01332</v>
+        <v>2.67561</v>
       </c>
       <c r="X4" s="5" t="n">
-        <v>2.05413</v>
+        <v>2.58377</v>
       </c>
       <c r="Y4" s="5" t="n">
-        <v>3.70195</v>
+        <v>2.16532</v>
       </c>
       <c r="Z4" s="5" t="n">
-        <v>1.86352</v>
+        <v>1.64847</v>
       </c>
       <c r="AA4" s="5" t="n">
-        <v>2.78189</v>
+        <v>2.58288</v>
       </c>
       <c r="AB4" s="5" t="n">
-        <v>2.54897</v>
+        <v>1.21223</v>
       </c>
       <c r="AC4" s="5" t="n">
-        <v>2.18696</v>
+        <v>3.69861</v>
       </c>
       <c r="AD4" s="5" t="n">
-        <v>2.68063</v>
+        <v>2.86373</v>
       </c>
       <c r="AE4" s="5" t="n">
-        <v>1.88682</v>
+        <v>1.58353</v>
       </c>
       <c r="AF4" s="5" t="n">
-        <v>3.92476</v>
+        <v>1.39618</v>
       </c>
       <c r="AG4" s="5" t="n">
-        <v>2.57617</v>
+        <v>1.60838</v>
       </c>
       <c r="AH4" s="5" t="n">
-        <v>5.79051</v>
+        <v>1.70735</v>
       </c>
       <c r="AI4" s="5" t="n">
-        <v>1.1642</v>
+        <v>1.2387</v>
       </c>
       <c r="AJ4" s="5" t="n">
-        <v>7.57999</v>
+        <v>1.38652</v>
       </c>
       <c r="AK4" s="5" t="n">
-        <v>1.39974</v>
+        <v>1.23585</v>
       </c>
       <c r="AL4" s="5" t="n">
-        <v>2.19238</v>
+        <v>1.30392</v>
       </c>
       <c r="AM4" s="5" t="n">
-        <v>3.81424</v>
+        <v>1.49789</v>
       </c>
       <c r="AN4" s="5" t="n">
-        <v>1.62149</v>
+        <v>1.19142</v>
       </c>
       <c r="AO4" s="5" t="n">
-        <v>2.56521</v>
+        <v>1.77277</v>
       </c>
       <c r="AP4" s="5" t="n">
-        <v>1.23031</v>
+        <v>2.118</v>
       </c>
       <c r="AQ4" s="5" t="n">
-        <v>2.08095</v>
+        <v>1.78133</v>
       </c>
       <c r="AR4" s="5" t="n">
-        <v>3.26521</v>
+        <v>1.03474</v>
       </c>
       <c r="AS4" s="5" t="n">
-        <v>6.62935</v>
+        <v>1.8391</v>
       </c>
       <c r="AT4" s="5" t="n">
-        <v>4.48527</v>
+        <v>1.6477</v>
       </c>
       <c r="AU4" s="5" t="n">
-        <v>3.94893</v>
+        <v>3.80214</v>
       </c>
       <c r="AV4" s="5" t="n">
-        <v>2.00075</v>
+        <v>1.35699</v>
       </c>
       <c r="AW4" s="5" t="n">
-        <v>1.67669</v>
+        <v>2.94584</v>
       </c>
       <c r="AX4" s="5" t="n">
-        <v>1.97765</v>
+        <v>1.28561</v>
       </c>
       <c r="AY4" s="5" t="n">
-        <v>2.04483</v>
+        <v>1.35271</v>
       </c>
       <c r="AZ4" s="5" t="n">
-        <v>2.32684</v>
+        <v>2.01492</v>
       </c>
       <c r="BA4" s="5" t="n">
-        <v>3.79995</v>
+        <v>1.3951</v>
       </c>
       <c r="BB4" s="5" t="n">
-        <v>1.78744</v>
+        <v>2.77402</v>
       </c>
       <c r="BC4" s="5" t="n">
-        <v>2.31834</v>
+        <v>1.36667</v>
       </c>
       <c r="BD4" s="5" t="n">
-        <v>1.33694</v>
+        <v>1.55504</v>
       </c>
       <c r="BE4" s="5" t="n">
-        <v>2.75064</v>
+        <v>1.6297</v>
       </c>
       <c r="BF4" s="5" t="n">
-        <v>1.49104</v>
+        <v>3.30919</v>
       </c>
       <c r="BG4" s="5" t="n">
-        <v>1.84709</v>
+        <v>1.36034</v>
       </c>
       <c r="BH4" s="5" t="n">
-        <v>2.48141</v>
+        <v>1.73352</v>
       </c>
       <c r="BI4" s="5" t="n">
-        <v>2.51129</v>
+        <v>1.49904</v>
       </c>
       <c r="BJ4" s="5" t="n">
-        <v>2.14227</v>
+        <v>1.19453</v>
       </c>
       <c r="BK4" s="5" t="n">
-        <v>2.91894</v>
+        <v>2.1005</v>
       </c>
       <c r="BL4" s="5" t="n">
-        <v>1.58682</v>
+        <v>1.21721</v>
       </c>
       <c r="BM4" s="5" t="n">
-        <v>1.28788</v>
+        <v>1.49537</v>
       </c>
       <c r="BN4" s="5" t="n">
-        <v>3.73464</v>
+        <v>5.38824</v>
       </c>
       <c r="BO4" s="5" t="n">
-        <v>2.71553</v>
+        <v>1.95126</v>
       </c>
       <c r="BP4" s="5" t="n">
-        <v>2.8673</v>
+        <v>3.3347</v>
       </c>
       <c r="BQ4" s="5" t="n">
-        <v>2.9567</v>
+        <v>1.66373</v>
       </c>
       <c r="BR4" s="5" t="n">
-        <v>4.01015</v>
+        <v>1.23208</v>
       </c>
       <c r="BS4" s="5" t="n">
-        <v>2.71206</v>
+        <v>4.39498</v>
       </c>
       <c r="BT4" s="5" t="n">
-        <v>4.55689</v>
+        <v>1.36953</v>
       </c>
       <c r="BU4" s="5" t="n">
-        <v>1.40103</v>
+        <v>1.44265</v>
       </c>
       <c r="BV4" s="5" t="n">
-        <v>1.43458</v>
+        <v>3.5613</v>
       </c>
       <c r="BW4" s="5" t="n">
-        <v>1.96092</v>
+        <v>2.98087</v>
       </c>
       <c r="BX4" s="5" t="n">
-        <v>1.43262</v>
+        <v>1.26343</v>
       </c>
       <c r="BY4" s="5" t="n">
-        <v>2.0939</v>
+        <v>1.89182</v>
       </c>
       <c r="BZ4" s="5" t="n">
-        <v>4.23299</v>
+        <v>2.59386</v>
       </c>
       <c r="CA4" s="5" t="n">
-        <v>1.83603</v>
+        <v>1.46032</v>
       </c>
       <c r="CB4" s="5" t="n">
-        <v>2.2362</v>
+        <v>2.35214</v>
       </c>
       <c r="CC4" s="5" t="n">
-        <v>3.70198</v>
+        <v>5.684</v>
       </c>
       <c r="CD4" s="5" t="n">
-        <v>1.8581</v>
+        <v>1.62216</v>
       </c>
       <c r="CE4" s="5" t="n">
-        <v>2.28343</v>
+        <v>6.7927</v>
       </c>
       <c r="CF4" s="5" t="n">
-        <v>4.51298</v>
+        <v>1.31625</v>
       </c>
       <c r="CG4" s="5" t="n">
-        <v>3.48752</v>
+        <v>1.33199</v>
       </c>
       <c r="CH4" s="5" t="n">
-        <v>1.60671</v>
+        <v>1.98993</v>
       </c>
       <c r="CI4" s="5" t="n">
-        <v>1.64581</v>
+        <v>1.62188</v>
       </c>
       <c r="CJ4" s="5" t="n">
-        <v>5.22899</v>
+        <v>2.48498</v>
       </c>
       <c r="CK4" s="5" t="n">
-        <v>1.62587</v>
+        <v>1.68676</v>
       </c>
       <c r="CL4" s="5" t="n">
-        <v>3.61425</v>
+        <v>1.41169</v>
       </c>
       <c r="CM4" s="5" t="n">
-        <v>2.06601</v>
+        <v>1.61665</v>
       </c>
       <c r="CN4" s="5" t="n">
-        <v>2.37734</v>
+        <v>1.75071</v>
       </c>
       <c r="CO4" s="5" t="n">
-        <v>1.75738</v>
+        <v>1.73114</v>
       </c>
       <c r="CP4" s="5" t="n">
-        <v>2.59383</v>
+        <v>1.26003</v>
       </c>
       <c r="CQ4" s="5" t="n">
-        <v>2.30825</v>
+        <v>1.19675</v>
       </c>
       <c r="CR4" s="5" t="n">
-        <v>3.19129</v>
+        <v>2.17955</v>
       </c>
       <c r="CS4" s="5" t="n">
-        <v>1.67723</v>
+        <v>2.37504</v>
       </c>
       <c r="CT4" s="5" t="n">
-        <v>3.06629</v>
+        <v>2.33334</v>
       </c>
       <c r="CU4" s="5" t="n">
-        <v>3.65611</v>
+        <v>2.00118</v>
       </c>
       <c r="CV4" s="5" t="n">
-        <v>2.3376</v>
+        <v>1.89327</v>
       </c>
       <c r="CW4" s="5" t="n">
-        <v>2.91194</v>
+        <v>1.50651</v>
       </c>
       <c r="CX4" s="5" t="n">
-        <v>1.98065</v>
+        <v>2.04433</v>
       </c>
       <c r="CY4" s="5" t="n">
-        <v>1.38016</v>
+        <v>1.29607</v>
       </c>
       <c r="CZ4" s="5" t="n">
-        <v>1.70257</v>
+        <v>1.55269</v>
       </c>
       <c r="DA4" s="5" t="n">
-        <v>3.41391</v>
+        <v>1.70313</v>
       </c>
       <c r="DB4" s="5" t="n">
-        <v>1.71998</v>
+        <v>1.79032</v>
       </c>
       <c r="DC4" s="5" t="n">
-        <v>1.72895</v>
+        <v>2.07977</v>
       </c>
       <c r="DD4" s="5" t="n">
-        <v>2.38039</v>
+        <v>4.07414</v>
       </c>
       <c r="DE4" s="5" t="n">
-        <v>4.37279</v>
+        <v>1.06791</v>
       </c>
       <c r="DF4" s="5" t="n">
-        <v>2.86276</v>
+        <v>1.20018</v>
       </c>
       <c r="DG4" s="5" t="n">
-        <v>1.25294</v>
+        <v>1.44697</v>
       </c>
       <c r="DH4" s="5" t="n">
-        <v>1.96704</v>
+        <v>3.11738</v>
       </c>
       <c r="DI4" s="5" t="n">
-        <v>3.46313</v>
+        <v>1.81499</v>
       </c>
       <c r="DJ4" s="5" t="n">
-        <v>3.19553</v>
+        <v>2.25489</v>
       </c>
       <c r="DK4" s="5" t="n">
-        <v>1.68196</v>
+        <v>1.2485</v>
       </c>
       <c r="DL4" s="5" t="n">
-        <v>1.24626</v>
+        <v>1.90219</v>
       </c>
       <c r="DM4" s="5" t="n">
-        <v>2.58207</v>
+        <v>3.54692</v>
       </c>
       <c r="DN4" s="5" t="n">
-        <v>2.20692</v>
+        <v>1.18776</v>
       </c>
       <c r="DO4" s="5" t="n">
-        <v>1.8493</v>
+        <v>1.87063</v>
       </c>
       <c r="DP4" s="5" t="n">
-        <v>1.38493</v>
+        <v>2.43444</v>
       </c>
       <c r="DQ4" s="5" t="n">
-        <v>7.43818</v>
+        <v>5.53944</v>
       </c>
       <c r="DR4" s="5" t="n">
-        <v>3.14865</v>
+        <v>2.78451</v>
       </c>
       <c r="DS4" s="5" t="n">
-        <v>1.95838</v>
+        <v>2.61532</v>
       </c>
       <c r="DT4" s="5" t="n">
-        <v>1.41481</v>
+        <v>1.85426</v>
       </c>
       <c r="DU4" s="5" t="n">
-        <v>7.26361</v>
+        <v>1.43371</v>
       </c>
       <c r="DV4" s="5" t="n">
-        <v>4.36773</v>
+        <v>1.65666</v>
       </c>
       <c r="DW4" s="5" t="n">
-        <v>2.89677</v>
+        <v>1.20779</v>
       </c>
       <c r="DX4" s="5" t="n">
-        <v>3.82751</v>
+        <v>2.03779</v>
       </c>
       <c r="DY4" s="5" t="n">
-        <v>1.75579</v>
+        <v>1.92128</v>
       </c>
       <c r="DZ4" s="5" t="n">
-        <v>5.10501</v>
+        <v>1.85409</v>
       </c>
       <c r="EA4" s="5" t="n">
-        <v>3.36353</v>
+        <v>1.46168</v>
       </c>
       <c r="EB4" s="5" t="n">
-        <v>4.19726</v>
+        <v>1.48915</v>
       </c>
       <c r="EC4" s="5" t="n">
-        <v>1.34525</v>
+        <v>1.27226</v>
       </c>
       <c r="ED4" s="5" t="n">
-        <v>3.46678</v>
+        <v>2.21329</v>
       </c>
       <c r="EE4" s="5" t="n">
-        <v>2.53524</v>
+        <v>1.55534</v>
       </c>
       <c r="EF4" s="5" t="n">
-        <v>2.42606</v>
+        <v>2.33163</v>
       </c>
       <c r="EG4" s="5" t="n">
-        <v>4.90711</v>
+        <v>2.04958</v>
       </c>
       <c r="EH4" s="5" t="n">
-        <v>4.67863</v>
+        <v>1.31845</v>
       </c>
       <c r="EI4" s="5" t="n">
-        <v>2.07217</v>
+        <v>2.12993</v>
       </c>
       <c r="EJ4" s="5" t="n">
-        <v>2.30115</v>
+        <v>1.96517</v>
       </c>
       <c r="EK4" s="5" t="n">
-        <v>1.92909</v>
+        <v>1.52472</v>
       </c>
       <c r="EL4" s="5" t="n">
-        <v>4.16069</v>
+        <v>2.43705</v>
       </c>
       <c r="EM4" s="5" t="n">
-        <v>3.78509</v>
+        <v>1.23334</v>
       </c>
       <c r="EN4" s="5" t="n">
-        <v>1.89889</v>
+        <v>1.94148</v>
       </c>
       <c r="EO4" s="5" t="n">
-        <v>1.53643</v>
+        <v>1.32172</v>
       </c>
       <c r="EP4" s="5" t="n">
-        <v>2.03499</v>
+        <v>1.85966</v>
       </c>
       <c r="EQ4" s="5" t="n">
-        <v>3.97043</v>
+        <v>1.45435</v>
       </c>
       <c r="ER4" s="5" t="n">
-        <v>1.36451</v>
+        <v>1.84487</v>
       </c>
       <c r="ES4" s="5" t="n">
-        <v>2.60916</v>
+        <v>2.49464</v>
       </c>
       <c r="ET4" s="5" t="n">
-        <v>3.3335</v>
+        <v>1.77624</v>
       </c>
       <c r="EU4" s="5" t="n">
-        <v>2.14707</v>
+        <v>2.61259</v>
       </c>
       <c r="EV4" s="5" t="n">
-        <v>2.23346</v>
+        <v>2.50878</v>
       </c>
       <c r="EW4" s="5" t="n">
-        <v>2.31601</v>
+        <v>1.1487</v>
       </c>
       <c r="EX4" s="5" t="n">
-        <v>1.40612</v>
+        <v>2.97675</v>
       </c>
       <c r="EY4" s="5" t="n">
-        <v>1.40015</v>
+        <v>2.49353</v>
       </c>
       <c r="EZ4" s="5" t="n">
-        <v>4.89448</v>
+        <v>1.99143</v>
       </c>
       <c r="FA4" s="5" t="n">
-        <v>2.19685</v>
+        <v>1.43499</v>
       </c>
       <c r="FB4" s="5" t="n">
-        <v>2.93166</v>
+        <v>2.19527</v>
       </c>
       <c r="FC4" s="5" t="n">
-        <v>1.52698</v>
+        <v>2.14658</v>
       </c>
       <c r="FD4" s="5" t="n">
-        <v>2.94052</v>
+        <v>1.45351</v>
       </c>
       <c r="FE4" s="5" t="n">
-        <v>2.51363</v>
+        <v>2.26781</v>
       </c>
       <c r="FF4" s="5" t="n">
-        <v>1.52734</v>
+        <v>4.30672</v>
       </c>
       <c r="FG4" s="5" t="n">
-        <v>1.67561</v>
+        <v>3.81076</v>
       </c>
       <c r="FH4" s="5" t="n">
-        <v>2.64518</v>
+        <v>1.1953</v>
       </c>
       <c r="FI4" s="5" t="n">
-        <v>1.42617</v>
+        <v>3.53473</v>
       </c>
       <c r="FJ4" s="5" t="n">
-        <v>9.1439</v>
+        <v>2.08489</v>
       </c>
       <c r="FK4" s="5" t="n">
-        <v>5.33416</v>
+        <v>1.84564</v>
       </c>
       <c r="FL4" s="5" t="n">
-        <v>1.51144</v>
+        <v>3.41601</v>
       </c>
       <c r="FM4" s="5" t="n">
-        <v>2.59808</v>
+        <v>1.35006</v>
       </c>
       <c r="FN4" s="5" t="n">
-        <v>2.58082</v>
+        <v>1.23886</v>
       </c>
       <c r="FO4" s="5" t="n">
-        <v>5.35691</v>
+        <v>1.53798</v>
       </c>
       <c r="FP4" s="5" t="n">
-        <v>3.92193</v>
+        <v>1.31285</v>
       </c>
       <c r="FQ4" s="5" t="n">
-        <v>2.74143</v>
+        <v>1.45437</v>
       </c>
       <c r="FR4" s="5" t="n">
-        <v>1.72706</v>
+        <v>2.09658</v>
       </c>
       <c r="FS4" s="5" t="n">
-        <v>3.07753</v>
+        <v>1.97778</v>
       </c>
       <c r="FT4" s="5" t="n">
-        <v>2.74586</v>
+        <v>1.10527</v>
       </c>
       <c r="FU4" s="5" t="n">
-        <v>1.59667</v>
+        <v>1.57974</v>
       </c>
       <c r="FV4" s="5" t="n">
-        <v>2.8457</v>
+        <v>1.43842</v>
       </c>
       <c r="FW4" s="5" t="n">
-        <v>4.77257</v>
+        <v>2.13727</v>
       </c>
       <c r="FX4" s="5" t="n">
-        <v>2.21847</v>
+        <v>1.63196</v>
       </c>
       <c r="FY4" s="5" t="n">
-        <v>1.99676</v>
+        <v>3.71236</v>
       </c>
       <c r="FZ4" s="5" t="n">
-        <v>2.52165</v>
+        <v>1.99803</v>
       </c>
       <c r="GA4" s="5" t="n">
-        <v>2.12707</v>
+        <v>2.31957</v>
       </c>
       <c r="GB4" s="5" t="n">
-        <v>4.95981</v>
+        <v>1.24303</v>
       </c>
       <c r="GC4" s="5" t="n">
-        <v>4.63012</v>
+        <v>2.07547</v>
       </c>
       <c r="GD4" s="5" t="n">
-        <v>1.22393</v>
+        <v>1.2259</v>
       </c>
       <c r="GE4" s="5" t="n">
-        <v>2.79874</v>
+        <v>2.51992</v>
       </c>
       <c r="GF4" s="5" t="n">
-        <v>1.66389</v>
+        <v>1.89002</v>
       </c>
       <c r="GG4" s="5" t="n">
-        <v>2.58529</v>
+        <v>1.11369</v>
       </c>
       <c r="GH4" s="5" t="n">
-        <v>2.31365</v>
+        <v>1.21086</v>
       </c>
       <c r="GI4" s="5" t="n">
-        <v>4.78579</v>
+        <v>1.78769</v>
       </c>
       <c r="GJ4" s="5" t="n">
-        <v>1.13969</v>
+        <v>1.15863</v>
       </c>
       <c r="GK4" s="5" t="n">
-        <v>3.13177</v>
+        <v>1.71036</v>
       </c>
       <c r="GL4" s="5" t="n">
-        <v>2.54754</v>
+        <v>1.65423</v>
       </c>
       <c r="GM4" s="5" t="n">
-        <v>1.46219</v>
+        <v>2.19427</v>
       </c>
       <c r="GN4" s="5" t="n">
-        <v>2.08677</v>
+        <v>2.53757</v>
       </c>
       <c r="GO4" s="5" t="n">
-        <v>4.29444</v>
+        <v>1.5611</v>
       </c>
       <c r="GP4" s="5" t="n">
-        <v>3.70335</v>
+        <v>2.11311</v>
       </c>
       <c r="GQ4" s="5" t="n">
-        <v>3.80642</v>
+        <v>4.23543</v>
       </c>
       <c r="GR4" s="5" t="n">
-        <v>3.64712</v>
+        <v>2.33701</v>
       </c>
       <c r="GS4" s="5" t="n">
-        <v>2.87767</v>
+        <v>4.49265</v>
       </c>
       <c r="GT4" s="5" t="n">
-        <v>1.75163</v>
+        <v>3.59781</v>
       </c>
       <c r="GU4" s="5" t="n">
-        <v>3.61355</v>
+        <v>2.80838</v>
       </c>
       <c r="GV4" s="5" t="n">
-        <v>4.91528</v>
+        <v>1.48564</v>
       </c>
       <c r="GW4" s="5" t="n">
-        <v>7.89927</v>
+        <v>1.52649</v>
       </c>
       <c r="GX4" s="5" t="n">
-        <v>1.98188</v>
+        <v>2.40667</v>
       </c>
       <c r="GY4" s="5" t="n">
-        <v>4.89339</v>
+        <v>1.86172</v>
       </c>
       <c r="GZ4" s="5" t="n">
-        <v>2.74787</v>
+        <v>3.2276</v>
       </c>
       <c r="HA4" s="5" t="n">
-        <v>7.45183</v>
+        <v>1.25993</v>
       </c>
       <c r="HB4" s="5" t="n">
-        <v>4.1188</v>
+        <v>1.39761</v>
       </c>
       <c r="HC4" s="5" t="n">
-        <v>2.19859</v>
+        <v>1.4986</v>
       </c>
       <c r="HD4" s="5" t="n">
-        <v>4.56203</v>
+        <v>1.84322</v>
       </c>
       <c r="HE4" s="5" t="n">
-        <v>1.98449</v>
+        <v>1.27916</v>
       </c>
       <c r="HF4" s="5" t="n">
-        <v>2.57329</v>
+        <v>1.60842</v>
       </c>
       <c r="HG4" s="5" t="n">
-        <v>2.67558</v>
+        <v>2.78423</v>
       </c>
       <c r="HH4" s="5" t="n">
-        <v>2.80708</v>
+        <v>2.09512</v>
       </c>
       <c r="HI4" s="5" t="n">
-        <v>3.20398</v>
+        <v>1.46978</v>
       </c>
       <c r="HJ4" s="5" t="n">
-        <v>5.15135</v>
+        <v>5.97424</v>
       </c>
       <c r="HK4" s="5" t="n">
-        <v>2.98769</v>
+        <v>1.54421</v>
       </c>
       <c r="HL4" s="5" t="n">
-        <v>2.11915</v>
+        <v>4.34657</v>
       </c>
       <c r="HM4" s="5" t="n">
-        <v>3.30334</v>
+        <v>1.32296</v>
       </c>
       <c r="HN4" s="5" t="n">
-        <v>2.42071</v>
+        <v>6.83881</v>
       </c>
       <c r="HO4" s="5" t="n">
-        <v>1.65988</v>
+        <v>1.9514</v>
       </c>
       <c r="HP4" s="5" t="n">
-        <v>1.57432</v>
+        <v>1.14084</v>
       </c>
       <c r="HQ4" s="5" t="n">
-        <v>1.51682</v>
+        <v>2.46889</v>
       </c>
       <c r="HR4" s="5" t="n">
-        <v>1.79842</v>
+        <v>2.09899</v>
       </c>
       <c r="HS4" s="5" t="n">
-        <v>3.14979</v>
+        <v>3.27456</v>
       </c>
       <c r="HT4" s="5" t="n">
-        <v>1.70439</v>
+        <v>3.20608</v>
       </c>
       <c r="HU4" s="5" t="n">
-        <v>1.43247</v>
+        <v>1.38825</v>
       </c>
       <c r="HV4" s="5" t="n">
-        <v>2.8622</v>
+        <v>3.60644</v>
       </c>
       <c r="HW4" s="5" t="n">
-        <v>1.82498</v>
+        <v>1.28235</v>
       </c>
       <c r="HX4" s="5" t="n">
-        <v>6.72184</v>
+        <v>2.28844</v>
       </c>
       <c r="HY4" s="5" t="n">
-        <v>1.71248</v>
+        <v>1.43835</v>
       </c>
       <c r="HZ4" s="5" t="n">
-        <v>2.9565</v>
+        <v>1.0623</v>
       </c>
       <c r="IA4" s="5" t="n">
-        <v>1.94893</v>
+        <v>1.22957</v>
       </c>
       <c r="IB4" s="5" t="n">
-        <v>2.15728</v>
+        <v>3.60138</v>
       </c>
       <c r="IC4" s="5" t="n">
-        <v>1.15337</v>
+        <v>1.73687</v>
       </c>
       <c r="ID4" s="5" t="n">
-        <v>1.75418</v>
+        <v>1.97136</v>
       </c>
       <c r="IE4" s="5" t="n">
-        <v>2.35089</v>
+        <v>2.60905</v>
       </c>
       <c r="IF4" s="5" t="n">
-        <v>1.83693</v>
+        <v>1.36148</v>
       </c>
       <c r="IG4" s="5" t="n">
-        <v>2.41868</v>
+        <v>1.48728</v>
       </c>
       <c r="IH4" s="5" t="n">
-        <v>1.74489</v>
+        <v>1.57211</v>
       </c>
       <c r="II4" s="5" t="n">
-        <v>2.79996</v>
+        <v>3.42241</v>
       </c>
       <c r="IJ4" s="5" t="n">
-        <v>4.10087</v>
+        <v>2.63626</v>
       </c>
       <c r="IK4" s="5" t="n">
-        <v>3.97463</v>
+        <v>2.22621</v>
       </c>
       <c r="IL4" s="5" t="n">
-        <v>3.04508</v>
+        <v>3.37867</v>
       </c>
       <c r="IM4" s="5" t="n">
-        <v>2.57715</v>
+        <v>1.84184</v>
       </c>
       <c r="IN4" s="5" t="n">
-        <v>3.85089</v>
+        <v>1.04369</v>
       </c>
       <c r="IO4" s="5" t="n">
-        <v>3.79292</v>
+        <v>2.38842</v>
       </c>
       <c r="IP4" s="5" t="n">
-        <v>2.76366</v>
+        <v>2.12372</v>
       </c>
       <c r="IQ4" s="5" t="n">
-        <v>2.21826</v>
+        <v>1.64788</v>
       </c>
       <c r="IR4" s="5" t="n">
-        <v>2.24304</v>
+        <v>2.02597</v>
       </c>
       <c r="IS4" s="5" t="n">
-        <v>1.69012</v>
+        <v>2.12383</v>
       </c>
       <c r="IT4" s="5" t="n">
-        <v>1.4482</v>
+        <v>1.83169</v>
       </c>
       <c r="IU4" s="5" t="n">
-        <v>2.37096</v>
+        <v>3.98216</v>
       </c>
       <c r="IV4" s="5" t="n">
-        <v>1.31122</v>
+        <v>1.8844</v>
       </c>
       <c r="IW4" s="5" t="n">
-        <v>5.98619</v>
+        <v>1.63163</v>
       </c>
       <c r="IX4" s="5" t="n">
-        <v>3.1715</v>
+        <v>3.15002</v>
       </c>
       <c r="IY4" s="5" t="n">
-        <v>2.31735</v>
+        <v>1.88392</v>
       </c>
       <c r="IZ4" s="5" t="n">
-        <v>1.6491</v>
+        <v>1.11762</v>
       </c>
       <c r="JA4" s="5" t="n">
-        <v>4.53755</v>
+        <v>2.70489</v>
       </c>
       <c r="JB4" s="5" t="n">
-        <v>2.33654</v>
+        <v>1.14236</v>
       </c>
       <c r="JC4" s="5"/>
       <c r="JD4" s="5"/>
@@ -8492,7 +8493,7 @@
       <c r="A12" s="12"/>
       <c r="B12" s="13" t="n">
         <f aca="false">AVERAGE(B3:B11)</f>
-        <v>7.71839834877735</v>
+        <v>7.64420622951523</v>
       </c>
       <c r="C12" s="13"/>
       <c r="D12" s="5"/>
@@ -8788,7 +8789,7 @@
       <c r="A13" s="12"/>
       <c r="B13" s="13" t="n">
         <f aca="false">_xlfn.STDEV.S(B3:B11)</f>
-        <v>5.93771475104144</v>
+        <v>6.01077715810034</v>
       </c>
       <c r="C13" s="13"/>
       <c r="D13" s="5"/>
@@ -10554,875 +10555,875 @@
       </c>
       <c r="B17" s="7" t="n">
         <f aca="false">AVERAGE(D17:AAA17)</f>
-        <v>68.4301109375</v>
+        <v>64.0331548611111</v>
       </c>
       <c r="C17" s="8" t="n">
         <f aca="false">_xlfn.STDEV.S(D17:AAB17)</f>
-        <v>81.1311329975171</v>
+        <v>72.8224634723933</v>
       </c>
       <c r="D17" s="5" t="n">
-        <v>13.4144</v>
+        <v>22.3688</v>
       </c>
       <c r="E17" s="5" t="n">
-        <v>36.4785</v>
+        <v>13.1343</v>
       </c>
       <c r="F17" s="5" t="n">
-        <v>7.51897</v>
+        <v>158.187</v>
       </c>
       <c r="G17" s="5" t="n">
-        <v>173.696</v>
+        <v>91.7537</v>
       </c>
       <c r="H17" s="5" t="n">
-        <v>21.8539</v>
+        <v>10.2159</v>
       </c>
       <c r="I17" s="5" t="n">
-        <v>25.0407</v>
+        <v>12.9739</v>
       </c>
       <c r="J17" s="5" t="n">
-        <v>48.5614</v>
+        <v>334.665</v>
       </c>
       <c r="K17" s="5" t="n">
-        <v>48.8884</v>
+        <v>39.5075</v>
       </c>
       <c r="L17" s="5" t="n">
-        <v>44.3248</v>
+        <v>64.8671</v>
       </c>
       <c r="M17" s="5" t="n">
-        <v>60.1875</v>
+        <v>196.795</v>
       </c>
       <c r="N17" s="5" t="n">
-        <v>14.8235</v>
+        <v>169.006</v>
       </c>
       <c r="O17" s="5" t="n">
-        <v>84.0407</v>
+        <v>21.3004</v>
       </c>
       <c r="P17" s="5" t="n">
-        <v>22.0025</v>
+        <v>75.5932</v>
       </c>
       <c r="Q17" s="5" t="n">
-        <v>8.6468</v>
+        <v>20.5207</v>
       </c>
       <c r="R17" s="5" t="n">
-        <v>28.3031</v>
+        <v>28.73</v>
       </c>
       <c r="S17" s="5" t="n">
-        <v>10.6462</v>
+        <v>29.2698</v>
       </c>
       <c r="T17" s="5" t="n">
-        <v>23.334</v>
+        <v>12.3613</v>
       </c>
       <c r="U17" s="5" t="n">
-        <v>71.3584</v>
+        <v>24.7421</v>
       </c>
       <c r="V17" s="5" t="n">
-        <v>9.08733</v>
+        <v>64.4242</v>
       </c>
       <c r="W17" s="5" t="n">
-        <v>53.2056</v>
+        <v>23.0175</v>
       </c>
       <c r="X17" s="5" t="n">
-        <v>8.80783</v>
+        <v>85.8843</v>
       </c>
       <c r="Y17" s="5" t="n">
-        <v>117.005</v>
+        <v>45.1114</v>
       </c>
       <c r="Z17" s="5" t="n">
-        <v>49.5563</v>
+        <v>16.841</v>
       </c>
       <c r="AA17" s="5" t="n">
-        <v>60.2042</v>
+        <v>11.0405</v>
       </c>
       <c r="AB17" s="5" t="n">
-        <v>17.5071</v>
+        <v>72.2112</v>
       </c>
       <c r="AC17" s="5" t="n">
-        <v>45.9023</v>
+        <v>12.7914</v>
       </c>
       <c r="AD17" s="5" t="n">
-        <v>14.6445</v>
+        <v>303.342</v>
       </c>
       <c r="AE17" s="5" t="n">
-        <v>55.7665</v>
+        <v>27.3073</v>
       </c>
       <c r="AF17" s="5" t="n">
-        <v>47.7981</v>
+        <v>58.0716</v>
       </c>
       <c r="AG17" s="5" t="n">
-        <v>14.4175</v>
+        <v>60.2289</v>
       </c>
       <c r="AH17" s="5" t="n">
-        <v>64.6614</v>
+        <v>62.9767</v>
       </c>
       <c r="AI17" s="5" t="n">
-        <v>174.32</v>
+        <v>223.69</v>
       </c>
       <c r="AJ17" s="5" t="n">
-        <v>58.5335</v>
+        <v>18.917</v>
       </c>
       <c r="AK17" s="5" t="n">
-        <v>70.4474</v>
+        <v>129.514</v>
       </c>
       <c r="AL17" s="5" t="n">
-        <v>66.6827</v>
+        <v>64.7793</v>
       </c>
       <c r="AM17" s="5" t="n">
-        <v>110.715</v>
+        <v>66.6949</v>
       </c>
       <c r="AN17" s="5" t="n">
-        <v>375.53</v>
+        <v>61.7894</v>
       </c>
       <c r="AO17" s="5" t="n">
-        <v>40.1685</v>
+        <v>145.839</v>
       </c>
       <c r="AP17" s="5" t="n">
-        <v>32.9201</v>
+        <v>29.815</v>
       </c>
       <c r="AQ17" s="5" t="n">
-        <v>13.121</v>
+        <v>53.4615</v>
       </c>
       <c r="AR17" s="5" t="n">
-        <v>176.123</v>
+        <v>19.407</v>
       </c>
       <c r="AS17" s="5" t="n">
-        <v>22.2891</v>
+        <v>118.18</v>
       </c>
       <c r="AT17" s="5" t="n">
-        <v>22.4413</v>
+        <v>140.508</v>
       </c>
       <c r="AU17" s="5" t="n">
-        <v>549.359</v>
+        <v>105.344</v>
       </c>
       <c r="AV17" s="5" t="n">
-        <v>66.4986</v>
+        <v>70.2796</v>
       </c>
       <c r="AW17" s="5" t="n">
-        <v>19.2657</v>
+        <v>58.0475</v>
       </c>
       <c r="AX17" s="5" t="n">
-        <v>47.1129</v>
+        <v>14.1807</v>
       </c>
       <c r="AY17" s="5" t="n">
-        <v>33.0251</v>
+        <v>21.1603</v>
       </c>
       <c r="AZ17" s="5" t="n">
-        <v>71.3401</v>
+        <v>61.1291</v>
       </c>
       <c r="BA17" s="5" t="n">
-        <v>22.3257</v>
+        <v>68.4835</v>
       </c>
       <c r="BB17" s="5" t="n">
-        <v>66.1878</v>
+        <v>82.6936</v>
       </c>
       <c r="BC17" s="5" t="n">
-        <v>25.6247</v>
+        <v>9.68612</v>
       </c>
       <c r="BD17" s="5" t="n">
-        <v>20.8339</v>
+        <v>54.9719</v>
       </c>
       <c r="BE17" s="5" t="n">
-        <v>161.305</v>
+        <v>16.8542</v>
       </c>
       <c r="BF17" s="5" t="n">
-        <v>189.483</v>
+        <v>249.003</v>
       </c>
       <c r="BG17" s="5" t="n">
-        <v>17.7074</v>
+        <v>63.6763</v>
       </c>
       <c r="BH17" s="5" t="n">
-        <v>266.06</v>
+        <v>15.7623</v>
       </c>
       <c r="BI17" s="5" t="n">
-        <v>229.068</v>
+        <v>145.332</v>
       </c>
       <c r="BJ17" s="5" t="n">
-        <v>12.2722</v>
+        <v>12.6539</v>
       </c>
       <c r="BK17" s="5" t="n">
-        <v>35.6937</v>
+        <v>19.0764</v>
       </c>
       <c r="BL17" s="5" t="n">
-        <v>72.0154</v>
+        <v>15.1732</v>
       </c>
       <c r="BM17" s="5" t="n">
-        <v>28.0412</v>
+        <v>83.7564</v>
       </c>
       <c r="BN17" s="5" t="n">
-        <v>103.32</v>
+        <v>21.4909</v>
       </c>
       <c r="BO17" s="5" t="n">
-        <v>57.6665</v>
+        <v>38.4504</v>
       </c>
       <c r="BP17" s="5" t="n">
-        <v>18.8764</v>
+        <v>238.697</v>
       </c>
       <c r="BQ17" s="5" t="n">
-        <v>12.334</v>
+        <v>62.4712</v>
       </c>
       <c r="BR17" s="5" t="n">
-        <v>60.3375</v>
+        <v>232.483</v>
       </c>
       <c r="BS17" s="5" t="n">
-        <v>26.782</v>
+        <v>125.252</v>
       </c>
       <c r="BT17" s="5" t="n">
-        <v>9.06921</v>
+        <v>24.9696</v>
       </c>
       <c r="BU17" s="5" t="n">
-        <v>60.9515</v>
+        <v>77.1994</v>
       </c>
       <c r="BV17" s="5" t="n">
-        <v>48.7264</v>
+        <v>69.6502</v>
       </c>
       <c r="BW17" s="5" t="n">
-        <v>250.935</v>
+        <v>146.85</v>
       </c>
       <c r="BX17" s="5" t="n">
-        <v>9.99762</v>
+        <v>76.2155</v>
       </c>
       <c r="BY17" s="5" t="n">
-        <v>36.8661</v>
+        <v>35.9683</v>
       </c>
       <c r="BZ17" s="5" t="n">
-        <v>59.7577</v>
+        <v>365.414</v>
       </c>
       <c r="CA17" s="5" t="n">
-        <v>25.0953</v>
+        <v>293.562</v>
       </c>
       <c r="CB17" s="5" t="n">
-        <v>47.7423</v>
+        <v>60.018</v>
       </c>
       <c r="CC17" s="5" t="n">
-        <v>11.8274</v>
+        <v>33.0022</v>
       </c>
       <c r="CD17" s="5" t="n">
-        <v>152.668</v>
+        <v>17.2117</v>
       </c>
       <c r="CE17" s="5" t="n">
-        <v>31.4416</v>
+        <v>20.0871</v>
       </c>
       <c r="CF17" s="5" t="n">
-        <v>29.092</v>
+        <v>19.2765</v>
       </c>
       <c r="CG17" s="5" t="n">
-        <v>33.2205</v>
+        <v>108.542</v>
       </c>
       <c r="CH17" s="5" t="n">
-        <v>157.97</v>
+        <v>18.4757</v>
       </c>
       <c r="CI17" s="5" t="n">
-        <v>27.8092</v>
+        <v>109.55</v>
       </c>
       <c r="CJ17" s="5" t="n">
-        <v>14.9254</v>
+        <v>76.753</v>
       </c>
       <c r="CK17" s="5" t="n">
-        <v>26.3352</v>
+        <v>22.8812</v>
       </c>
       <c r="CL17" s="5" t="n">
-        <v>52.8954</v>
+        <v>69.615</v>
       </c>
       <c r="CM17" s="5" t="n">
-        <v>298.409</v>
+        <v>61.1391</v>
       </c>
       <c r="CN17" s="5" t="n">
-        <v>11.5779</v>
+        <v>130.7</v>
       </c>
       <c r="CO17" s="5" t="n">
-        <v>72.0966</v>
+        <v>61.3773</v>
       </c>
       <c r="CP17" s="5" t="n">
-        <v>51.99</v>
+        <v>14.6823</v>
       </c>
       <c r="CQ17" s="5" t="n">
-        <v>86.5065</v>
+        <v>18.0761</v>
       </c>
       <c r="CR17" s="5" t="n">
-        <v>92.9238</v>
+        <v>30.238</v>
       </c>
       <c r="CS17" s="5" t="n">
-        <v>19.8661</v>
+        <v>19.2165</v>
       </c>
       <c r="CT17" s="5" t="n">
-        <v>37.6623</v>
+        <v>58.818</v>
       </c>
       <c r="CU17" s="5" t="n">
-        <v>56.1586</v>
+        <v>62.8861</v>
       </c>
       <c r="CV17" s="5" t="n">
-        <v>21.9283</v>
+        <v>69.2768</v>
       </c>
       <c r="CW17" s="5" t="n">
-        <v>61.9397</v>
+        <v>32.3277</v>
       </c>
       <c r="CX17" s="5" t="n">
-        <v>22.2674</v>
+        <v>67.5711</v>
       </c>
       <c r="CY17" s="5" t="n">
-        <v>36.052</v>
+        <v>27.8049</v>
       </c>
       <c r="CZ17" s="5" t="n">
-        <v>27.0829</v>
+        <v>26.9944</v>
       </c>
       <c r="DA17" s="5" t="n">
-        <v>23.092</v>
+        <v>16.9129</v>
       </c>
       <c r="DB17" s="5" t="n">
-        <v>17.901</v>
+        <v>36.8988</v>
       </c>
       <c r="DC17" s="5" t="n">
-        <v>16.7269</v>
+        <v>209.43</v>
       </c>
       <c r="DD17" s="5" t="n">
-        <v>68.0012</v>
+        <v>98.0526</v>
       </c>
       <c r="DE17" s="5" t="n">
-        <v>187.855</v>
+        <v>30.5229</v>
       </c>
       <c r="DF17" s="5" t="n">
-        <v>131.401</v>
+        <v>20.0693</v>
       </c>
       <c r="DG17" s="5" t="n">
-        <v>64.1369</v>
+        <v>63.7568</v>
       </c>
       <c r="DH17" s="5" t="n">
-        <v>22.8942</v>
+        <v>52.1173</v>
       </c>
       <c r="DI17" s="5" t="n">
-        <v>33.4503</v>
+        <v>28.7764</v>
       </c>
       <c r="DJ17" s="5" t="n">
-        <v>65.6093</v>
+        <v>496.693</v>
       </c>
       <c r="DK17" s="5" t="n">
-        <v>59.0739</v>
+        <v>56.7361</v>
       </c>
       <c r="DL17" s="5" t="n">
-        <v>19.6935</v>
+        <v>233.747</v>
       </c>
       <c r="DM17" s="5" t="n">
-        <v>20.6521</v>
+        <v>216.535</v>
       </c>
       <c r="DN17" s="5" t="n">
-        <v>11.0576</v>
+        <v>69.3374</v>
       </c>
       <c r="DO17" s="5" t="n">
-        <v>67.6573</v>
+        <v>44.1049</v>
       </c>
       <c r="DP17" s="5" t="n">
-        <v>351.197</v>
+        <v>22.1647</v>
       </c>
       <c r="DQ17" s="5" t="n">
-        <v>51.2274</v>
+        <v>12.137</v>
       </c>
       <c r="DR17" s="5" t="n">
-        <v>66.7532</v>
+        <v>342.837</v>
       </c>
       <c r="DS17" s="5" t="n">
-        <v>42.7361</v>
+        <v>11.9512</v>
       </c>
       <c r="DT17" s="5" t="n">
-        <v>14.3813</v>
+        <v>59.0684</v>
       </c>
       <c r="DU17" s="5" t="n">
-        <v>65.4507</v>
+        <v>32.6118</v>
       </c>
       <c r="DV17" s="5" t="n">
-        <v>13.9391</v>
+        <v>177.117</v>
       </c>
       <c r="DW17" s="5" t="n">
-        <v>67.3248</v>
+        <v>15.6187</v>
       </c>
       <c r="DX17" s="5" t="n">
-        <v>20.0718</v>
+        <v>10.2983</v>
       </c>
       <c r="DY17" s="5" t="n">
-        <v>56.2661</v>
+        <v>60.5343</v>
       </c>
       <c r="DZ17" s="5" t="n">
-        <v>20.1397</v>
+        <v>114.791</v>
       </c>
       <c r="EA17" s="5" t="n">
-        <v>14.305</v>
+        <v>17.4938</v>
       </c>
       <c r="EB17" s="5" t="n">
-        <v>12.221</v>
+        <v>59.115</v>
       </c>
       <c r="EC17" s="5" t="n">
-        <v>113.562</v>
+        <v>26.2885</v>
       </c>
       <c r="ED17" s="5" t="n">
-        <v>98.1554</v>
+        <v>159.632</v>
       </c>
       <c r="EE17" s="5" t="n">
-        <v>16.8975</v>
+        <v>14.9153</v>
       </c>
       <c r="EF17" s="5" t="n">
-        <v>68.1013</v>
+        <v>38.1952</v>
       </c>
       <c r="EG17" s="5" t="n">
-        <v>163.831</v>
+        <v>158.985</v>
       </c>
       <c r="EH17" s="5" t="n">
-        <v>72.6342</v>
+        <v>40.5393</v>
       </c>
       <c r="EI17" s="5" t="n">
-        <v>14.1369</v>
+        <v>24.3718</v>
       </c>
       <c r="EJ17" s="5" t="n">
-        <v>56.1324</v>
+        <v>23.406</v>
       </c>
       <c r="EK17" s="5" t="n">
-        <v>187.866</v>
+        <v>81.5534</v>
       </c>
       <c r="EL17" s="5" t="n">
-        <v>156.376</v>
+        <v>64.3368</v>
       </c>
       <c r="EM17" s="5" t="n">
-        <v>25.976</v>
+        <v>82.5446</v>
       </c>
       <c r="EN17" s="5" t="n">
-        <v>50.6593</v>
+        <v>40.0155</v>
       </c>
       <c r="EO17" s="5" t="n">
-        <v>14.6907</v>
+        <v>55.3211</v>
       </c>
       <c r="EP17" s="5" t="n">
-        <v>21.0532</v>
+        <v>60.3157</v>
       </c>
       <c r="EQ17" s="5" t="n">
-        <v>250.847</v>
+        <v>29.4726</v>
       </c>
       <c r="ER17" s="5" t="n">
-        <v>15.8216</v>
+        <v>64.9629</v>
       </c>
       <c r="ES17" s="5" t="n">
-        <v>344.209</v>
+        <v>26.7744</v>
       </c>
       <c r="ET17" s="5" t="n">
-        <v>25.465</v>
+        <v>39.1081</v>
       </c>
       <c r="EU17" s="5" t="n">
-        <v>220.289</v>
+        <v>60.9129</v>
       </c>
       <c r="EV17" s="5" t="n">
-        <v>28.7828</v>
+        <v>53.8191</v>
       </c>
       <c r="EW17" s="5" t="n">
-        <v>61.8904</v>
+        <v>14.1541</v>
       </c>
       <c r="EX17" s="5" t="n">
-        <v>398.312</v>
+        <v>44.1213</v>
       </c>
       <c r="EY17" s="5" t="n">
-        <v>14.3111</v>
+        <v>14.2521</v>
       </c>
       <c r="EZ17" s="5" t="n">
-        <v>22.188</v>
+        <v>26.236</v>
       </c>
       <c r="FA17" s="5" t="n">
-        <v>157.278</v>
+        <v>10.0246</v>
       </c>
       <c r="FB17" s="5" t="n">
-        <v>15.3496</v>
+        <v>37.0348</v>
       </c>
       <c r="FC17" s="5" t="n">
-        <v>174.432</v>
+        <v>15.1671</v>
       </c>
       <c r="FD17" s="5" t="n">
-        <v>61.5319</v>
+        <v>10.9614</v>
       </c>
       <c r="FE17" s="5" t="n">
-        <v>13.4443</v>
+        <v>41.6038</v>
       </c>
       <c r="FF17" s="5" t="n">
-        <v>267.107</v>
+        <v>52.1401</v>
       </c>
       <c r="FG17" s="5" t="n">
-        <v>74.5795</v>
+        <v>13.2014</v>
       </c>
       <c r="FH17" s="5" t="n">
-        <v>15.8684</v>
+        <v>389.068</v>
       </c>
       <c r="FI17" s="5" t="n">
-        <v>58.8521</v>
+        <v>45.2735</v>
       </c>
       <c r="FJ17" s="5" t="n">
-        <v>79.1278</v>
+        <v>15.7652</v>
       </c>
       <c r="FK17" s="5" t="n">
-        <v>91.3546</v>
+        <v>54.2032</v>
       </c>
       <c r="FL17" s="5" t="n">
-        <v>77.004</v>
+        <v>38.1861</v>
       </c>
       <c r="FM17" s="5" t="n">
-        <v>35.2404</v>
+        <v>26.5911</v>
       </c>
       <c r="FN17" s="5" t="n">
-        <v>63.3759</v>
+        <v>70.1998</v>
       </c>
       <c r="FO17" s="5" t="n">
-        <v>89.0743</v>
+        <v>95.9855</v>
       </c>
       <c r="FP17" s="5" t="n">
-        <v>16.438</v>
+        <v>25.7089</v>
       </c>
       <c r="FQ17" s="5" t="n">
-        <v>115.62</v>
+        <v>15.4697</v>
       </c>
       <c r="FR17" s="5" t="n">
-        <v>78.8839</v>
+        <v>51.3641</v>
       </c>
       <c r="FS17" s="5" t="n">
-        <v>17.033</v>
+        <v>53.9814</v>
       </c>
       <c r="FT17" s="5" t="n">
-        <v>15.4078</v>
+        <v>53.8427</v>
       </c>
       <c r="FU17" s="5" t="n">
-        <v>269.738</v>
+        <v>10.099</v>
       </c>
       <c r="FV17" s="5" t="n">
-        <v>247.308</v>
+        <v>24.7244</v>
       </c>
       <c r="FW17" s="5" t="n">
-        <v>33.128</v>
+        <v>32.5922</v>
       </c>
       <c r="FX17" s="5" t="n">
-        <v>141.376</v>
+        <v>25.3724</v>
       </c>
       <c r="FY17" s="5" t="n">
-        <v>108.881</v>
+        <v>41.7097</v>
       </c>
       <c r="FZ17" s="5" t="n">
-        <v>274.15</v>
+        <v>11.3808</v>
       </c>
       <c r="GA17" s="5" t="n">
-        <v>65.8951</v>
+        <v>19.3752</v>
       </c>
       <c r="GB17" s="5" t="n">
-        <v>50.4045</v>
+        <v>69.9099</v>
       </c>
       <c r="GC17" s="5" t="n">
-        <v>59.868</v>
+        <v>14.1884</v>
       </c>
       <c r="GD17" s="5" t="n">
-        <v>21.8089</v>
+        <v>20.1049</v>
       </c>
       <c r="GE17" s="5" t="n">
-        <v>55.8014</v>
+        <v>38.6382</v>
       </c>
       <c r="GF17" s="5" t="n">
-        <v>28.5592</v>
+        <v>38.2285</v>
       </c>
       <c r="GG17" s="5" t="n">
-        <v>67.7078</v>
+        <v>7.79612</v>
       </c>
       <c r="GH17" s="5" t="n">
-        <v>13.375</v>
+        <v>8.27049</v>
       </c>
       <c r="GI17" s="5" t="n">
-        <v>199.157</v>
+        <v>125.286</v>
       </c>
       <c r="GJ17" s="5" t="n">
-        <v>289.454</v>
+        <v>137.364</v>
       </c>
       <c r="GK17" s="5" t="n">
-        <v>14.3626</v>
+        <v>13.8154</v>
       </c>
       <c r="GL17" s="5" t="n">
-        <v>20.3712</v>
+        <v>35.9774</v>
       </c>
       <c r="GM17" s="5" t="n">
-        <v>61.4011</v>
+        <v>102.63</v>
       </c>
       <c r="GN17" s="5" t="n">
-        <v>55.1919</v>
+        <v>23.9473</v>
       </c>
       <c r="GO17" s="5" t="n">
-        <v>11.4068</v>
+        <v>45.0153</v>
       </c>
       <c r="GP17" s="5" t="n">
-        <v>25.9471</v>
+        <v>10.0851</v>
       </c>
       <c r="GQ17" s="5" t="n">
-        <v>18.6067</v>
+        <v>16.9161</v>
       </c>
       <c r="GR17" s="5" t="n">
-        <v>16.7819</v>
+        <v>16.7008</v>
       </c>
       <c r="GS17" s="5" t="n">
-        <v>59.7132</v>
+        <v>50.9103</v>
       </c>
       <c r="GT17" s="5" t="n">
-        <v>46.8901</v>
+        <v>12.8125</v>
       </c>
       <c r="GU17" s="5" t="n">
-        <v>57.159</v>
+        <v>8.07324</v>
       </c>
       <c r="GV17" s="5" t="n">
-        <v>46.2971</v>
+        <v>8.88244</v>
       </c>
       <c r="GW17" s="5" t="n">
-        <v>49.2816</v>
+        <v>45.3713</v>
       </c>
       <c r="GX17" s="5" t="n">
-        <v>69.792</v>
+        <v>20.7263</v>
       </c>
       <c r="GY17" s="5" t="n">
-        <v>25.0928</v>
+        <v>21.478</v>
       </c>
       <c r="GZ17" s="5" t="n">
-        <v>42.1369</v>
+        <v>38.3867</v>
       </c>
       <c r="HA17" s="5" t="n">
-        <v>66.6616</v>
+        <v>12.0352</v>
       </c>
       <c r="HB17" s="5" t="n">
-        <v>63.1902</v>
+        <v>17.9681</v>
       </c>
       <c r="HC17" s="5" t="n">
-        <v>34.5604</v>
+        <v>17.4847</v>
       </c>
       <c r="HD17" s="5" t="n">
-        <v>176.34</v>
+        <v>47.6427</v>
       </c>
       <c r="HE17" s="5" t="n">
-        <v>58.6167</v>
+        <v>14.7272</v>
       </c>
       <c r="HF17" s="5" t="n">
-        <v>66.0283</v>
+        <v>215.465</v>
       </c>
       <c r="HG17" s="5" t="n">
-        <v>30.1205</v>
+        <v>20.3852</v>
       </c>
       <c r="HH17" s="5" t="n">
-        <v>35.3084</v>
+        <v>236.333</v>
       </c>
       <c r="HI17" s="5" t="n">
-        <v>87.8624</v>
+        <v>134.318</v>
       </c>
       <c r="HJ17" s="5" t="n">
-        <v>85.6536</v>
+        <v>20.5287</v>
       </c>
       <c r="HK17" s="5" t="n">
-        <v>15.5574</v>
+        <v>55.1777</v>
       </c>
       <c r="HL17" s="5" t="n">
-        <v>38.2743</v>
+        <v>9.80811</v>
       </c>
       <c r="HM17" s="5" t="n">
-        <v>59.5543</v>
+        <v>62.4467</v>
       </c>
       <c r="HN17" s="5" t="n">
-        <v>67.5301</v>
+        <v>23.6357</v>
       </c>
       <c r="HO17" s="5" t="n">
-        <v>73.84</v>
+        <v>11.7295</v>
       </c>
       <c r="HP17" s="5" t="n">
-        <v>23.1654</v>
+        <v>179.718</v>
       </c>
       <c r="HQ17" s="5" t="n">
-        <v>59.4981</v>
+        <v>17.3783</v>
       </c>
       <c r="HR17" s="5" t="n">
-        <v>25.6497</v>
+        <v>13.5979</v>
       </c>
       <c r="HS17" s="5" t="n">
-        <v>18.787</v>
+        <v>27.1804</v>
       </c>
       <c r="HT17" s="5" t="n">
-        <v>57.2531</v>
+        <v>62.7685</v>
       </c>
       <c r="HU17" s="5" t="n">
-        <v>186.313</v>
+        <v>35.881</v>
       </c>
       <c r="HV17" s="5" t="n">
-        <v>32.4175</v>
+        <v>12.9835</v>
       </c>
       <c r="HW17" s="5" t="n">
-        <v>12.1068</v>
+        <v>208.62</v>
       </c>
       <c r="HX17" s="5" t="n">
-        <v>28.5444</v>
+        <v>51.6269</v>
       </c>
       <c r="HY17" s="5" t="n">
-        <v>111.017</v>
+        <v>26.4349</v>
       </c>
       <c r="HZ17" s="5" t="n">
-        <v>16.0422</v>
+        <v>38.853</v>
       </c>
       <c r="IA17" s="5" t="n">
-        <v>202.004</v>
+        <v>87.1117</v>
       </c>
       <c r="IB17" s="5" t="n">
-        <v>94.5942</v>
+        <v>33.1182</v>
       </c>
       <c r="IC17" s="5" t="n">
-        <v>21.4096</v>
+        <v>209.582</v>
       </c>
       <c r="ID17" s="5" t="n">
-        <v>25.4526</v>
+        <v>63.6534</v>
       </c>
       <c r="IE17" s="5" t="n">
-        <v>28.3035</v>
+        <v>9.96858</v>
       </c>
       <c r="IF17" s="5" t="n">
-        <v>25.4732</v>
+        <v>50.9462</v>
       </c>
       <c r="IG17" s="5" t="n">
-        <v>16.1113</v>
+        <v>38.8884</v>
       </c>
       <c r="IH17" s="5" t="n">
-        <v>31.5708</v>
+        <v>57.093</v>
       </c>
       <c r="II17" s="5" t="n">
-        <v>12.7683</v>
+        <v>48.9206</v>
       </c>
       <c r="IJ17" s="5" t="n">
-        <v>17.6179</v>
+        <v>23.4661</v>
       </c>
       <c r="IK17" s="5" t="n">
-        <v>7.07942</v>
+        <v>84.6454</v>
       </c>
       <c r="IL17" s="5" t="n">
-        <v>13.9321</v>
+        <v>8.3452</v>
       </c>
       <c r="IM17" s="5" t="n">
-        <v>16.3935</v>
+        <v>31.3386</v>
       </c>
       <c r="IN17" s="5" t="n">
-        <v>66.2411</v>
+        <v>29.2846</v>
       </c>
       <c r="IO17" s="5" t="n">
-        <v>73.1388</v>
+        <v>47.4493</v>
       </c>
       <c r="IP17" s="5" t="n">
-        <v>21.5018</v>
+        <v>22.9652</v>
       </c>
       <c r="IQ17" s="5" t="n">
-        <v>31.2417</v>
+        <v>47.5809</v>
       </c>
       <c r="IR17" s="5" t="n">
-        <v>51.693</v>
+        <v>16.3736</v>
       </c>
       <c r="IS17" s="5" t="n">
-        <v>15.0377</v>
+        <v>23.7252</v>
       </c>
       <c r="IT17" s="5" t="n">
-        <v>45.6613</v>
+        <v>44.6415</v>
       </c>
       <c r="IU17" s="5" t="n">
-        <v>16.5919</v>
+        <v>31.1805</v>
       </c>
       <c r="IV17" s="5" t="n">
-        <v>54.9018</v>
+        <v>63.0373</v>
       </c>
       <c r="IW17" s="5" t="n">
-        <v>26.4625</v>
+        <v>16.3883</v>
       </c>
       <c r="IX17" s="5" t="n">
-        <v>16.7539</v>
+        <v>89.15</v>
       </c>
       <c r="IY17" s="5" t="n">
-        <v>44.797</v>
+        <v>26.2483</v>
       </c>
       <c r="IZ17" s="5" t="n">
-        <v>36.4798</v>
+        <v>47.489</v>
       </c>
       <c r="JA17" s="5" t="n">
-        <v>56.4357</v>
+        <v>52.2094</v>
       </c>
       <c r="JB17" s="5" t="n">
-        <v>95.9675</v>
+        <v>52.9126</v>
       </c>
       <c r="JC17" s="5" t="n">
-        <v>9.64647</v>
+        <v>16.1422</v>
       </c>
       <c r="JD17" s="5" t="n">
-        <v>35.1775</v>
+        <v>196.681</v>
       </c>
       <c r="JE17" s="5" t="n">
-        <v>12.8735</v>
+        <v>138.572</v>
       </c>
       <c r="JF17" s="5" t="n">
-        <v>13.5939</v>
+        <v>16.9497</v>
       </c>
       <c r="JG17" s="5" t="n">
-        <v>24.145</v>
+        <v>79.3769</v>
       </c>
       <c r="JH17" s="5" t="n">
-        <v>15.5057</v>
+        <v>10.6718</v>
       </c>
       <c r="JI17" s="5" t="n">
-        <v>38.0249</v>
+        <v>46.1097</v>
       </c>
       <c r="JJ17" s="5" t="n">
-        <v>14.6106</v>
+        <v>49.2966</v>
       </c>
       <c r="JK17" s="5" t="n">
-        <v>56.3739</v>
+        <v>20.0722</v>
       </c>
       <c r="JL17" s="5" t="n">
-        <v>102.928</v>
+        <v>30.4987</v>
       </c>
       <c r="JM17" s="5" t="n">
-        <v>83.9022</v>
+        <v>10.1068</v>
       </c>
       <c r="JN17" s="5" t="n">
-        <v>13.0682</v>
+        <v>10.897</v>
       </c>
       <c r="JO17" s="5" t="n">
-        <v>24.7174</v>
+        <v>72.0257</v>
       </c>
       <c r="JP17" s="5" t="n">
-        <v>71.6351</v>
+        <v>11.4649</v>
       </c>
       <c r="JQ17" s="5" t="n">
-        <v>64.1916</v>
+        <v>18.4433</v>
       </c>
       <c r="JR17" s="5" t="n">
-        <v>23.048</v>
+        <v>23.8499</v>
       </c>
       <c r="JS17" s="5" t="n">
-        <v>45.0927</v>
+        <v>180.128</v>
       </c>
       <c r="JT17" s="5" t="n">
-        <v>55.4386</v>
+        <v>59.0783</v>
       </c>
       <c r="JU17" s="5" t="n">
-        <v>186.534</v>
+        <v>81.3986</v>
       </c>
       <c r="JV17" s="5" t="n">
-        <v>572.489</v>
+        <v>57.971</v>
       </c>
       <c r="JW17" s="5" t="n">
-        <v>31.9058</v>
+        <v>365.496</v>
       </c>
       <c r="JX17" s="5" t="n">
-        <v>78.2156</v>
+        <v>18.3911</v>
       </c>
       <c r="JY17" s="5" t="n">
-        <v>22.947</v>
+        <v>61.8233</v>
       </c>
       <c r="JZ17" s="5" t="n">
-        <v>16.5434</v>
+        <v>11.8368</v>
       </c>
       <c r="KA17" s="5" t="n">
-        <v>55.4689</v>
+        <v>30.1668</v>
       </c>
       <c r="KB17" s="5" t="n">
-        <v>260.267</v>
+        <v>218.806</v>
       </c>
       <c r="KC17" s="5" t="n">
-        <v>40.6028</v>
+        <v>65.8745</v>
       </c>
       <c r="KD17" s="5" t="n">
-        <v>234.857</v>
+        <v>27.9039</v>
       </c>
       <c r="KE17" s="5" t="n">
-        <v>35.8125</v>
+        <v>58.5788</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -17567,13 +17568,13 @@
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B25" s="13" t="n">
         <f aca="false">AVERAGE(B16:B24)</f>
-        <v>17.9640160300926</v>
+        <v>17.4754653549383</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B26" s="13" t="n">
         <f aca="false">_xlfn.STDEV.S(B16:B24)</f>
-        <v>21.5418713260399</v>
+        <v>20.2663774617892</v>
       </c>
     </row>
   </sheetData>
@@ -17590,4 +17591,27 @@
     <oddFooter/>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetData/>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;Kffffff&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;KffffffPage &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>